<commit_message>
Excel corregido con ID's y hoja de participantes
</commit_message>
<xml_diff>
--- a/horarios.xlsx
+++ b/horarios.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Horarios" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Participantes" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -473,7 +474,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -505,12 +506,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -520,7 +521,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -537,22 +538,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -569,27 +570,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(16,)]</t>
         </is>
       </c>
     </row>
@@ -611,17 +612,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
     </row>
@@ -633,7 +634,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Sin participantes']</t>
+          <t>[(15,)]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,17 +644,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['Sin participantes']</t>
+          <t>[(15,)]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>['Sin participantes']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',)]</t>
+          <t>[(15,)]</t>
         </is>
       </c>
     </row>
@@ -665,7 +666,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(15,), (16,)]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,7 +676,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',), ('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(15,), (14,), (16,)]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -685,7 +686,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[('samuel.ceballos4453@alumnos.udg.mx',), ('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(15,), (14,)]</t>
         </is>
       </c>
     </row>
@@ -697,17 +698,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(15,), (16,)]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',)]</t>
+          <t>[(14,)]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(15,), (16,)]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -717,7 +718,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['Sin participantes']</t>
+          <t>[(15,)]</t>
         </is>
       </c>
     </row>
@@ -729,7 +730,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(16,)]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -739,7 +740,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[('franco.silva4477@alumnos.udg.mx',), ('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(14,), (16,)]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -781,7 +782,128 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[('juan.ortega4533@alumnos.udg.mx',)]</t>
+          <t>[(16,)]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Apellidos</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Correo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Teléfono</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>JUAN JOSE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ORTEGA MORALES</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>juan.ortega4533@alumnos.udg.mx</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3322445566</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SAMUEL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CEBALLOS MURGUIA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>samuel.ceballos4453@alumnos.udg.mx</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>3311111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FRANCO EDUARDO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SILVA CHACÓN</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>franco.silva4477@alumnos.udg.mx</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3355669988</t>
         </is>
       </c>
     </row>

</xml_diff>